<commit_message>
IFT test scripts added with payroll
</commit_message>
<xml_diff>
--- a/src/test/java/com/corpnet/testData/Transaction_Tracker/Transaction_Tracker.xlsx
+++ b/src/test/java/com/corpnet/testData/Transaction_Tracker/Transaction_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\BBLCorpnetappAutomation\src\test\java\com\corpnet\testData\Transaction_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9153510-253C-4EC4-8715-0192114A72B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AED6B06-7856-4C46-B544-1E35D371F72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="77">
   <si>
     <t>Transaction Reference</t>
   </si>
@@ -253,13 +253,10 @@
     <t>IFT_Payroll</t>
   </si>
   <si>
-    <t>140823172821487P</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>220823130144443P</t>
+    <t>240823105137288P</t>
   </si>
 </sst>
 </file>
@@ -708,24 +705,66 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -744,21 +783,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -770,33 +794,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1081,10 +1078,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,20 +1102,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="79"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="93"/>
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:15" ht="63" x14ac:dyDescent="0.25">
@@ -1169,17 +1166,17 @@
       <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="82" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="54"/>
       <c r="G3" s="13"/>
@@ -1189,7 +1186,7 @@
       <c r="K3" s="18"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1198,8 +1195,8 @@
       <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="72"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="48" t="s">
         <v>6</v>
       </c>
@@ -1219,8 +1216,8 @@
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="72"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="90"/>
       <c r="D5" s="49" t="s">
         <v>7</v>
       </c>
@@ -1240,8 +1237,8 @@
       <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="72"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="90"/>
       <c r="D6" s="48" t="s">
         <v>74</v>
       </c>
@@ -1261,8 +1258,8 @@
       <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="86"/>
-      <c r="C7" s="72"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="90"/>
       <c r="D7" s="48" t="s">
         <v>56</v>
       </c>
@@ -1282,8 +1279,8 @@
       <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="73"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="48" t="s">
         <v>55</v>
       </c>
@@ -1303,8 +1300,8 @@
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="71" t="s">
+      <c r="B9" s="85"/>
+      <c r="C9" s="82" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="49" t="s">
@@ -1326,8 +1323,8 @@
       <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="86"/>
-      <c r="C10" s="72"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="90"/>
       <c r="D10" s="48" t="s">
         <v>6</v>
       </c>
@@ -1347,8 +1344,8 @@
       <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="86"/>
-      <c r="C11" s="72"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="90"/>
       <c r="D11" s="49" t="s">
         <v>7</v>
       </c>
@@ -1366,8 +1363,8 @@
       <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="86"/>
-      <c r="C12" s="72"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="48" t="s">
         <v>8</v>
       </c>
@@ -1387,8 +1384,8 @@
       <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="48" t="s">
         <v>56</v>
       </c>
@@ -1408,8 +1405,8 @@
       <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="86"/>
-      <c r="C14" s="73"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="83"/>
       <c r="D14" s="48" t="s">
         <v>55</v>
       </c>
@@ -1429,8 +1426,8 @@
       <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="86"/>
-      <c r="C15" s="71" t="s">
+      <c r="B15" s="85"/>
+      <c r="C15" s="82" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="48" t="s">
@@ -1452,50 +1449,50 @@
       <c r="A16" s="10">
         <v>14</v>
       </c>
-      <c r="B16" s="86"/>
-      <c r="C16" s="72"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="90"/>
       <c r="D16" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="80"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="90"/>
-      <c r="I16" s="90"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="90"/>
-      <c r="L16" s="83"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="99"/>
+      <c r="I16" s="99"/>
+      <c r="J16" s="99"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="71"/>
       <c r="M16" s="44"/>
-      <c r="N16" s="83"/>
+      <c r="N16" s="71"/>
       <c r="O16" s="44"/>
     </row>
     <row r="17" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
-      <c r="B17" s="86"/>
-      <c r="C17" s="72"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="80"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="84"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="100"/>
+      <c r="J17" s="100"/>
+      <c r="K17" s="100"/>
+      <c r="L17" s="72"/>
       <c r="M17" s="45"/>
-      <c r="N17" s="84"/>
+      <c r="N17" s="72"/>
       <c r="O17" s="45"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>16</v>
       </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="72"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="90"/>
       <c r="D18" s="48" t="s">
         <v>8</v>
       </c>
@@ -1515,8 +1512,8 @@
       <c r="A19" s="10">
         <v>17</v>
       </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="72"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="48" t="s">
         <v>56</v>
       </c>
@@ -1536,8 +1533,8 @@
       <c r="A20" s="10">
         <v>18</v>
       </c>
-      <c r="B20" s="86"/>
-      <c r="C20" s="73"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="83"/>
       <c r="D20" s="48" t="s">
         <v>55</v>
       </c>
@@ -1557,7 +1554,7 @@
       <c r="A21" s="10">
         <v>19</v>
       </c>
-      <c r="B21" s="87"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="4"/>
       <c r="D21" s="48"/>
       <c r="E21" s="32"/>
@@ -1576,10 +1573,10 @@
       <c r="A22" s="10">
         <v>20</v>
       </c>
-      <c r="B22" s="85" t="s">
+      <c r="B22" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="82" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="48" t="s">
@@ -1603,8 +1600,8 @@
       <c r="A23" s="10">
         <v>21</v>
       </c>
-      <c r="B23" s="86"/>
-      <c r="C23" s="72"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="49" t="s">
         <v>4</v>
       </c>
@@ -1624,8 +1621,8 @@
       <c r="A24" s="10">
         <v>22</v>
       </c>
-      <c r="B24" s="86"/>
-      <c r="C24" s="72"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="90"/>
       <c r="D24" s="48" t="s">
         <v>37</v>
       </c>
@@ -1645,8 +1642,8 @@
       <c r="A25" s="10">
         <v>23</v>
       </c>
-      <c r="B25" s="86"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="90"/>
       <c r="D25" s="48" t="s">
         <v>38</v>
       </c>
@@ -1666,8 +1663,8 @@
       <c r="A26" s="10">
         <v>24</v>
       </c>
-      <c r="B26" s="86"/>
-      <c r="C26" s="72"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="90"/>
       <c r="D26" s="48" t="s">
         <v>56</v>
       </c>
@@ -1687,8 +1684,8 @@
       <c r="A27" s="10">
         <v>25</v>
       </c>
-      <c r="B27" s="86"/>
-      <c r="C27" s="73"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="83"/>
       <c r="D27" s="48" t="s">
         <v>55</v>
       </c>
@@ -1708,8 +1705,8 @@
       <c r="A28" s="10">
         <v>26</v>
       </c>
-      <c r="B28" s="86"/>
-      <c r="C28" s="71" t="s">
+      <c r="B28" s="85"/>
+      <c r="C28" s="82" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="49" t="s">
@@ -1731,8 +1728,8 @@
       <c r="A29" s="10">
         <v>27</v>
       </c>
-      <c r="B29" s="86"/>
-      <c r="C29" s="72"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="90"/>
       <c r="D29" s="48" t="s">
         <v>4</v>
       </c>
@@ -1752,8 +1749,8 @@
       <c r="A30" s="10">
         <v>28</v>
       </c>
-      <c r="B30" s="86"/>
-      <c r="C30" s="72"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="90"/>
       <c r="D30" s="48" t="s">
         <v>37</v>
       </c>
@@ -1773,8 +1770,8 @@
       <c r="A31" s="10">
         <v>29</v>
       </c>
-      <c r="B31" s="86"/>
-      <c r="C31" s="73"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="83"/>
       <c r="D31" s="48" t="s">
         <v>38</v>
       </c>
@@ -1794,8 +1791,8 @@
       <c r="A32" s="10">
         <v>30</v>
       </c>
-      <c r="B32" s="86"/>
-      <c r="C32" s="71" t="s">
+      <c r="B32" s="85"/>
+      <c r="C32" s="82" t="s">
         <v>46</v>
       </c>
       <c r="D32" s="48" t="s">
@@ -1817,8 +1814,8 @@
       <c r="A33" s="10">
         <v>31</v>
       </c>
-      <c r="B33" s="86"/>
-      <c r="C33" s="72"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="90"/>
       <c r="D33" s="48" t="s">
         <v>37</v>
       </c>
@@ -1838,8 +1835,8 @@
       <c r="A34" s="10">
         <v>32</v>
       </c>
-      <c r="B34" s="87"/>
-      <c r="C34" s="73"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="83"/>
       <c r="D34" s="48" t="s">
         <v>38</v>
       </c>
@@ -1860,7 +1857,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="23"/>
-      <c r="C35" s="71" t="s">
+      <c r="C35" s="82" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="48" t="s">
@@ -1883,7 +1880,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="23"/>
-      <c r="C36" s="73"/>
+      <c r="C36" s="83"/>
       <c r="D36" s="48" t="s">
         <v>55</v>
       </c>
@@ -1903,10 +1900,10 @@
       <c r="A37" s="10">
         <v>35</v>
       </c>
-      <c r="B37" s="74" t="s">
+      <c r="B37" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="71" t="s">
+      <c r="C37" s="82" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="49" t="s">
@@ -1928,8 +1925,8 @@
       <c r="A38" s="10">
         <v>36</v>
       </c>
-      <c r="B38" s="75"/>
-      <c r="C38" s="72"/>
+      <c r="B38" s="88"/>
+      <c r="C38" s="90"/>
       <c r="D38" s="48" t="s">
         <v>19</v>
       </c>
@@ -1949,8 +1946,8 @@
       <c r="A39" s="10">
         <v>37</v>
       </c>
-      <c r="B39" s="75"/>
-      <c r="C39" s="73"/>
+      <c r="B39" s="88"/>
+      <c r="C39" s="83"/>
       <c r="D39" s="48" t="s">
         <v>55</v>
       </c>
@@ -1970,8 +1967,8 @@
       <c r="A40" s="10">
         <v>38</v>
       </c>
-      <c r="B40" s="75"/>
-      <c r="C40" s="71" t="s">
+      <c r="B40" s="88"/>
+      <c r="C40" s="82" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="49" t="s">
@@ -1993,8 +1990,8 @@
       <c r="A41" s="10">
         <v>39</v>
       </c>
-      <c r="B41" s="75"/>
-      <c r="C41" s="72"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="90"/>
       <c r="D41" s="48" t="s">
         <v>19</v>
       </c>
@@ -2014,8 +2011,8 @@
       <c r="A42" s="10">
         <v>40</v>
       </c>
-      <c r="B42" s="76"/>
-      <c r="C42" s="73"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="83"/>
       <c r="D42" s="48" t="s">
         <v>55</v>
       </c>
@@ -2054,10 +2051,10 @@
       <c r="A44" s="10">
         <v>42</v>
       </c>
-      <c r="B44" s="74" t="s">
+      <c r="B44" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="71" t="s">
+      <c r="C44" s="82" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="49" t="s">
@@ -2079,8 +2076,8 @@
       <c r="A45" s="10">
         <v>43</v>
       </c>
-      <c r="B45" s="75"/>
-      <c r="C45" s="73"/>
+      <c r="B45" s="88"/>
+      <c r="C45" s="83"/>
       <c r="D45" s="48" t="s">
         <v>55</v>
       </c>
@@ -2100,8 +2097,8 @@
       <c r="A46" s="10">
         <v>44</v>
       </c>
-      <c r="B46" s="75"/>
-      <c r="C46" s="71" t="s">
+      <c r="B46" s="88"/>
+      <c r="C46" s="82" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="49" t="s">
@@ -2123,8 +2120,8 @@
       <c r="A47" s="10">
         <v>45</v>
       </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="72"/>
+      <c r="B47" s="88"/>
+      <c r="C47" s="90"/>
       <c r="D47" s="49" t="s">
         <v>71</v>
       </c>
@@ -2144,8 +2141,8 @@
       <c r="A48" s="10">
         <v>46</v>
       </c>
-      <c r="B48" s="75"/>
-      <c r="C48" s="73"/>
+      <c r="B48" s="88"/>
+      <c r="C48" s="83"/>
       <c r="D48" s="48" t="s">
         <v>55</v>
       </c>
@@ -2165,8 +2162,8 @@
       <c r="A49" s="10">
         <v>47</v>
       </c>
-      <c r="B49" s="75"/>
-      <c r="C49" s="71" t="s">
+      <c r="B49" s="88"/>
+      <c r="C49" s="82" t="s">
         <v>24</v>
       </c>
       <c r="D49" s="49" t="s">
@@ -2188,8 +2185,8 @@
       <c r="A50" s="10">
         <v>48</v>
       </c>
-      <c r="B50" s="75"/>
-      <c r="C50" s="72"/>
+      <c r="B50" s="88"/>
+      <c r="C50" s="90"/>
       <c r="D50" s="49" t="s">
         <v>26</v>
       </c>
@@ -2209,8 +2206,8 @@
       <c r="A51" s="10">
         <v>49</v>
       </c>
-      <c r="B51" s="75"/>
-      <c r="C51" s="73"/>
+      <c r="B51" s="88"/>
+      <c r="C51" s="83"/>
       <c r="D51" s="48" t="s">
         <v>55</v>
       </c>
@@ -2230,8 +2227,8 @@
       <c r="A52" s="10">
         <v>50</v>
       </c>
-      <c r="B52" s="75"/>
-      <c r="C52" s="71" t="s">
+      <c r="B52" s="88"/>
+      <c r="C52" s="82" t="s">
         <v>27</v>
       </c>
       <c r="D52" s="48" t="s">
@@ -2253,8 +2250,8 @@
       <c r="A53" s="10">
         <v>51</v>
       </c>
-      <c r="B53" s="76"/>
-      <c r="C53" s="73"/>
+      <c r="B53" s="89"/>
+      <c r="C53" s="83"/>
       <c r="D53" s="48" t="s">
         <v>29</v>
       </c>
@@ -2293,7 +2290,7 @@
       <c r="A55" s="10">
         <v>53</v>
       </c>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="73" t="s">
         <v>30</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -2318,7 +2315,7 @@
       <c r="A56" s="10">
         <v>54</v>
       </c>
-      <c r="B56" s="93"/>
+      <c r="B56" s="74"/>
       <c r="C56" s="7" t="s">
         <v>33</v>
       </c>
@@ -2341,7 +2338,7 @@
       <c r="A57" s="10">
         <v>55</v>
       </c>
-      <c r="B57" s="93"/>
+      <c r="B57" s="74"/>
       <c r="C57" s="7" t="s">
         <v>35</v>
       </c>
@@ -2364,7 +2361,7 @@
       <c r="A58" s="10">
         <v>56</v>
       </c>
-      <c r="B58" s="94"/>
+      <c r="B58" s="75"/>
       <c r="C58" s="25"/>
       <c r="D58" s="48" t="s">
         <v>55</v>
@@ -2385,10 +2382,10 @@
       <c r="A59" s="10">
         <v>57</v>
       </c>
-      <c r="B59" s="92" t="s">
+      <c r="B59" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="C59" s="71" t="s">
+      <c r="C59" s="82" t="s">
         <v>4</v>
       </c>
       <c r="D59" s="48" t="s">
@@ -2410,8 +2407,8 @@
       <c r="A60" s="10">
         <v>58</v>
       </c>
-      <c r="B60" s="93"/>
-      <c r="C60" s="73"/>
+      <c r="B60" s="74"/>
+      <c r="C60" s="83"/>
       <c r="D60" s="48" t="s">
         <v>60</v>
       </c>
@@ -2430,7 +2427,7 @@
       <c r="A61" s="10">
         <v>59</v>
       </c>
-      <c r="B61" s="93"/>
+      <c r="B61" s="74"/>
       <c r="C61" s="27" t="s">
         <v>37</v>
       </c>
@@ -2453,7 +2450,7 @@
       <c r="A62" s="10">
         <v>60</v>
       </c>
-      <c r="B62" s="93"/>
+      <c r="B62" s="74"/>
       <c r="C62" s="27" t="s">
         <v>38</v>
       </c>
@@ -2476,7 +2473,7 @@
       <c r="A63" s="10">
         <v>61</v>
       </c>
-      <c r="B63" s="93"/>
+      <c r="B63" s="74"/>
       <c r="C63" s="25"/>
       <c r="D63" s="48" t="s">
         <v>56</v>
@@ -2497,7 +2494,7 @@
       <c r="A64" s="10">
         <v>62</v>
       </c>
-      <c r="B64" s="94"/>
+      <c r="B64" s="75"/>
       <c r="C64" s="25"/>
       <c r="D64" s="48" t="s">
         <v>55</v>
@@ -2518,7 +2515,7 @@
       <c r="A65" s="10">
         <v>63</v>
       </c>
-      <c r="B65" s="92" t="s">
+      <c r="B65" s="73" t="s">
         <v>41</v>
       </c>
       <c r="C65" s="27" t="s">
@@ -2528,7 +2525,7 @@
         <v>7</v>
       </c>
       <c r="E65" s="38"/>
-      <c r="F65" s="95"/>
+      <c r="F65" s="76"/>
       <c r="G65" s="9"/>
       <c r="H65" s="18"/>
       <c r="I65" s="18"/>
@@ -2543,7 +2540,7 @@
       <c r="A66" s="10">
         <v>64</v>
       </c>
-      <c r="B66" s="93"/>
+      <c r="B66" s="74"/>
       <c r="C66" s="27" t="s">
         <v>37</v>
       </c>
@@ -2551,7 +2548,7 @@
         <v>7</v>
       </c>
       <c r="E66" s="38"/>
-      <c r="F66" s="96"/>
+      <c r="F66" s="77"/>
       <c r="G66" s="9"/>
       <c r="H66" s="18"/>
       <c r="I66" s="18"/>
@@ -2566,7 +2563,7 @@
       <c r="A67" s="10">
         <v>65</v>
       </c>
-      <c r="B67" s="93"/>
+      <c r="B67" s="74"/>
       <c r="C67" s="27" t="s">
         <v>38</v>
       </c>
@@ -2574,7 +2571,7 @@
         <v>7</v>
       </c>
       <c r="E67" s="38"/>
-      <c r="F67" s="97"/>
+      <c r="F67" s="78"/>
       <c r="G67" s="9"/>
       <c r="H67" s="18"/>
       <c r="I67" s="18"/>
@@ -2589,7 +2586,7 @@
       <c r="A68" s="10">
         <v>66</v>
       </c>
-      <c r="B68" s="93"/>
+      <c r="B68" s="74"/>
       <c r="C68" s="25"/>
       <c r="D68" s="48" t="s">
         <v>56</v>
@@ -2610,7 +2607,7 @@
       <c r="A69" s="10">
         <v>67</v>
       </c>
-      <c r="B69" s="94"/>
+      <c r="B69" s="75"/>
       <c r="C69" s="25"/>
       <c r="D69" s="48" t="s">
         <v>55</v>
@@ -2631,7 +2628,7 @@
       <c r="A70" s="10">
         <v>68</v>
       </c>
-      <c r="B70" s="92" t="s">
+      <c r="B70" s="73" t="s">
         <v>42</v>
       </c>
       <c r="C70" s="28" t="s">
@@ -2656,7 +2653,7 @@
       <c r="A71" s="10">
         <v>69</v>
       </c>
-      <c r="B71" s="93"/>
+      <c r="B71" s="74"/>
       <c r="C71" s="28" t="s">
         <v>37</v>
       </c>
@@ -2679,7 +2676,7 @@
       <c r="A72" s="10">
         <v>70</v>
       </c>
-      <c r="B72" s="93"/>
+      <c r="B72" s="74"/>
       <c r="C72" s="28" t="s">
         <v>38</v>
       </c>
@@ -2702,7 +2699,7 @@
       <c r="A73" s="10">
         <v>71</v>
       </c>
-      <c r="B73" s="93"/>
+      <c r="B73" s="74"/>
       <c r="C73" s="24"/>
       <c r="D73" s="48" t="s">
         <v>56</v>
@@ -2723,7 +2720,7 @@
       <c r="A74" s="10">
         <v>72</v>
       </c>
-      <c r="B74" s="94"/>
+      <c r="B74" s="75"/>
       <c r="C74" s="26"/>
       <c r="D74" s="48" t="s">
         <v>55</v>
@@ -2744,7 +2741,7 @@
       <c r="A75" s="10">
         <v>73</v>
       </c>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="73" t="s">
         <v>61</v>
       </c>
       <c r="C75" s="7" t="s">
@@ -2769,7 +2766,7 @@
       <c r="A76" s="10">
         <v>74</v>
       </c>
-      <c r="B76" s="93"/>
+      <c r="B76" s="74"/>
       <c r="C76" s="7" t="s">
         <v>63</v>
       </c>
@@ -2792,7 +2789,7 @@
       <c r="A77" s="10">
         <v>75</v>
       </c>
-      <c r="B77" s="93"/>
+      <c r="B77" s="74"/>
       <c r="C77" s="43"/>
       <c r="D77" s="49" t="s">
         <v>69</v>
@@ -2813,7 +2810,7 @@
       <c r="A78" s="10">
         <v>76</v>
       </c>
-      <c r="B78" s="94"/>
+      <c r="B78" s="75"/>
       <c r="C78" s="25"/>
       <c r="D78" s="48" t="s">
         <v>55</v>
@@ -2834,7 +2831,7 @@
       <c r="A79" s="10">
         <v>77</v>
       </c>
-      <c r="B79" s="92" t="s">
+      <c r="B79" s="73" t="s">
         <v>47</v>
       </c>
       <c r="C79" s="7" t="s">
@@ -2844,7 +2841,7 @@
         <v>66</v>
       </c>
       <c r="E79" s="38"/>
-      <c r="F79" s="95"/>
+      <c r="F79" s="76"/>
       <c r="G79" s="9"/>
       <c r="H79" s="18"/>
       <c r="I79" s="18"/>
@@ -2859,7 +2856,7 @@
       <c r="A80" s="10">
         <v>78</v>
       </c>
-      <c r="B80" s="93"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="7" t="s">
         <v>57</v>
       </c>
@@ -2867,7 +2864,7 @@
         <v>66</v>
       </c>
       <c r="E80" s="38"/>
-      <c r="F80" s="96"/>
+      <c r="F80" s="77"/>
       <c r="G80" s="9"/>
       <c r="H80" s="18"/>
       <c r="I80" s="18"/>
@@ -2882,7 +2879,7 @@
       <c r="A81" s="10">
         <v>79</v>
       </c>
-      <c r="B81" s="93"/>
+      <c r="B81" s="74"/>
       <c r="C81" s="7" t="s">
         <v>54</v>
       </c>
@@ -2890,7 +2887,7 @@
         <v>66</v>
       </c>
       <c r="E81" s="38"/>
-      <c r="F81" s="97"/>
+      <c r="F81" s="78"/>
       <c r="G81" s="9"/>
       <c r="H81" s="18"/>
       <c r="I81" s="18"/>
@@ -2905,7 +2902,7 @@
       <c r="A82" s="10">
         <v>80</v>
       </c>
-      <c r="B82" s="94"/>
+      <c r="B82" s="75"/>
       <c r="C82" s="7" t="s">
         <v>65</v>
       </c>
@@ -2928,7 +2925,7 @@
       <c r="A83" s="10">
         <v>81</v>
       </c>
-      <c r="B83" s="98" t="s">
+      <c r="B83" s="79" t="s">
         <v>48</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -2953,7 +2950,7 @@
       <c r="A84" s="10">
         <v>82</v>
       </c>
-      <c r="B84" s="99"/>
+      <c r="B84" s="80"/>
       <c r="C84" s="4" t="s">
         <v>52</v>
       </c>
@@ -2976,7 +2973,7 @@
       <c r="A85" s="10">
         <v>83</v>
       </c>
-      <c r="B85" s="100"/>
+      <c r="B85" s="81"/>
       <c r="C85" s="4" t="s">
         <v>53</v>
       </c>
@@ -3001,6 +2998,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="B3:B21"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C15:C20"/>
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="B75:B78"/>
     <mergeCell ref="B79:B82"/>
@@ -3017,27 +3035,6 @@
     <mergeCell ref="B44:B53"/>
     <mergeCell ref="C52:C53"/>
     <mergeCell ref="C22:C27"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="B3:B21"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="C46:C48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
IF test scripts added with payroll
</commit_message>
<xml_diff>
--- a/src/test/java/com/corpnet/testData/Transaction_Tracker/Transaction_Tracker.xlsx
+++ b/src/test/java/com/corpnet/testData/Transaction_Tracker/Transaction_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\BBLCorpnetappAutomation\src\test\java\com\corpnet\testData\Transaction_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AED6B06-7856-4C46-B544-1E35D371F72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68558409-3F47-46E3-BB19-A951B923CA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="79">
   <si>
     <t>Transaction Reference</t>
   </si>
@@ -253,10 +253,16 @@
     <t>IFT_Payroll</t>
   </si>
   <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>1501200131929001</t>
+  </si>
+  <si>
+    <t>290823125923414P</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>240823105137288P</t>
   </si>
 </sst>
 </file>
@@ -705,12 +711,69 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -737,63 +800,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1081,7 +1087,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,20 +1108,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="93"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="79"/>
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:15" ht="63" x14ac:dyDescent="0.25">
@@ -1166,19 +1172,19 @@
       <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="71" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3"/>
+      <c r="F3" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="54"/>
       <c r="G3" s="13"/>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
@@ -1195,8 +1201,8 @@
       <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="90"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="48" t="s">
         <v>6</v>
       </c>
@@ -1216,8 +1222,8 @@
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="90"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="49" t="s">
         <v>7</v>
       </c>
@@ -1237,8 +1243,8 @@
       <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="90"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="48" t="s">
         <v>74</v>
       </c>
@@ -1258,8 +1264,8 @@
       <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="90"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="48" t="s">
         <v>56</v>
       </c>
@@ -1279,8 +1285,8 @@
       <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="83"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="73"/>
       <c r="D8" s="48" t="s">
         <v>55</v>
       </c>
@@ -1300,8 +1306,8 @@
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="82" t="s">
+      <c r="B9" s="86"/>
+      <c r="C9" s="71" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="49" t="s">
@@ -1323,12 +1329,14 @@
       <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="90"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="72"/>
       <c r="D10" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="42"/>
+      <c r="E10" s="42" t="s">
+        <v>77</v>
+      </c>
       <c r="F10" s="42"/>
       <c r="G10" s="13"/>
       <c r="H10" s="18"/>
@@ -1336,7 +1344,9 @@
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="M10" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
@@ -1344,8 +1354,8 @@
       <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="90"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="49" t="s">
         <v>7</v>
       </c>
@@ -1363,8 +1373,8 @@
       <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="85"/>
-      <c r="C12" s="90"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="48" t="s">
         <v>8</v>
       </c>
@@ -1384,8 +1394,8 @@
       <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="85"/>
-      <c r="C13" s="90"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="48" t="s">
         <v>56</v>
       </c>
@@ -1405,8 +1415,8 @@
       <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="83"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="48" t="s">
         <v>55</v>
       </c>
@@ -1426,8 +1436,8 @@
       <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="85"/>
-      <c r="C15" s="82" t="s">
+      <c r="B15" s="86"/>
+      <c r="C15" s="71" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="48" t="s">
@@ -1449,50 +1459,50 @@
       <c r="A16" s="10">
         <v>14</v>
       </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="90"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="72"/>
       <c r="D16" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="94"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="71"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="88"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
+      <c r="L16" s="83"/>
       <c r="M16" s="44"/>
-      <c r="N16" s="71"/>
+      <c r="N16" s="83"/>
       <c r="O16" s="44"/>
     </row>
     <row r="17" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="90"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="72"/>
       <c r="D17" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="94"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="100"/>
-      <c r="J17" s="100"/>
-      <c r="K17" s="100"/>
-      <c r="L17" s="72"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="91"/>
+      <c r="J17" s="91"/>
+      <c r="K17" s="91"/>
+      <c r="L17" s="84"/>
       <c r="M17" s="45"/>
-      <c r="N17" s="72"/>
+      <c r="N17" s="84"/>
       <c r="O17" s="45"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>16</v>
       </c>
-      <c r="B18" s="85"/>
-      <c r="C18" s="90"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="48" t="s">
         <v>8</v>
       </c>
@@ -1512,8 +1522,8 @@
       <c r="A19" s="10">
         <v>17</v>
       </c>
-      <c r="B19" s="85"/>
-      <c r="C19" s="90"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="72"/>
       <c r="D19" s="48" t="s">
         <v>56</v>
       </c>
@@ -1533,8 +1543,8 @@
       <c r="A20" s="10">
         <v>18</v>
       </c>
-      <c r="B20" s="85"/>
-      <c r="C20" s="83"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="73"/>
       <c r="D20" s="48" t="s">
         <v>55</v>
       </c>
@@ -1554,7 +1564,7 @@
       <c r="A21" s="10">
         <v>19</v>
       </c>
-      <c r="B21" s="86"/>
+      <c r="B21" s="87"/>
       <c r="C21" s="4"/>
       <c r="D21" s="48"/>
       <c r="E21" s="32"/>
@@ -1573,10 +1583,10 @@
       <c r="A22" s="10">
         <v>20</v>
       </c>
-      <c r="B22" s="84" t="s">
+      <c r="B22" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="82" t="s">
+      <c r="C22" s="71" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="48" t="s">
@@ -1600,8 +1610,8 @@
       <c r="A23" s="10">
         <v>21</v>
       </c>
-      <c r="B23" s="85"/>
-      <c r="C23" s="90"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="72"/>
       <c r="D23" s="49" t="s">
         <v>4</v>
       </c>
@@ -1621,8 +1631,8 @@
       <c r="A24" s="10">
         <v>22</v>
       </c>
-      <c r="B24" s="85"/>
-      <c r="C24" s="90"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="48" t="s">
         <v>37</v>
       </c>
@@ -1642,8 +1652,8 @@
       <c r="A25" s="10">
         <v>23</v>
       </c>
-      <c r="B25" s="85"/>
-      <c r="C25" s="90"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="72"/>
       <c r="D25" s="48" t="s">
         <v>38</v>
       </c>
@@ -1663,8 +1673,8 @@
       <c r="A26" s="10">
         <v>24</v>
       </c>
-      <c r="B26" s="85"/>
-      <c r="C26" s="90"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="72"/>
       <c r="D26" s="48" t="s">
         <v>56</v>
       </c>
@@ -1684,8 +1694,8 @@
       <c r="A27" s="10">
         <v>25</v>
       </c>
-      <c r="B27" s="85"/>
-      <c r="C27" s="83"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="73"/>
       <c r="D27" s="48" t="s">
         <v>55</v>
       </c>
@@ -1705,8 +1715,8 @@
       <c r="A28" s="10">
         <v>26</v>
       </c>
-      <c r="B28" s="85"/>
-      <c r="C28" s="82" t="s">
+      <c r="B28" s="86"/>
+      <c r="C28" s="71" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="49" t="s">
@@ -1728,8 +1738,8 @@
       <c r="A29" s="10">
         <v>27</v>
       </c>
-      <c r="B29" s="85"/>
-      <c r="C29" s="90"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="72"/>
       <c r="D29" s="48" t="s">
         <v>4</v>
       </c>
@@ -1749,8 +1759,8 @@
       <c r="A30" s="10">
         <v>28</v>
       </c>
-      <c r="B30" s="85"/>
-      <c r="C30" s="90"/>
+      <c r="B30" s="86"/>
+      <c r="C30" s="72"/>
       <c r="D30" s="48" t="s">
         <v>37</v>
       </c>
@@ -1770,8 +1780,8 @@
       <c r="A31" s="10">
         <v>29</v>
       </c>
-      <c r="B31" s="85"/>
-      <c r="C31" s="83"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="48" t="s">
         <v>38</v>
       </c>
@@ -1791,8 +1801,8 @@
       <c r="A32" s="10">
         <v>30</v>
       </c>
-      <c r="B32" s="85"/>
-      <c r="C32" s="82" t="s">
+      <c r="B32" s="86"/>
+      <c r="C32" s="71" t="s">
         <v>46</v>
       </c>
       <c r="D32" s="48" t="s">
@@ -1814,8 +1824,8 @@
       <c r="A33" s="10">
         <v>31</v>
       </c>
-      <c r="B33" s="85"/>
-      <c r="C33" s="90"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="72"/>
       <c r="D33" s="48" t="s">
         <v>37</v>
       </c>
@@ -1835,8 +1845,8 @@
       <c r="A34" s="10">
         <v>32</v>
       </c>
-      <c r="B34" s="86"/>
-      <c r="C34" s="83"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="73"/>
       <c r="D34" s="48" t="s">
         <v>38</v>
       </c>
@@ -1857,7 +1867,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="23"/>
-      <c r="C35" s="82" t="s">
+      <c r="C35" s="71" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="48" t="s">
@@ -1880,7 +1890,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="23"/>
-      <c r="C36" s="83"/>
+      <c r="C36" s="73"/>
       <c r="D36" s="48" t="s">
         <v>55</v>
       </c>
@@ -1900,10 +1910,10 @@
       <c r="A37" s="10">
         <v>35</v>
       </c>
-      <c r="B37" s="87" t="s">
+      <c r="B37" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="82" t="s">
+      <c r="C37" s="71" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="49" t="s">
@@ -1925,8 +1935,8 @@
       <c r="A38" s="10">
         <v>36</v>
       </c>
-      <c r="B38" s="88"/>
-      <c r="C38" s="90"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="72"/>
       <c r="D38" s="48" t="s">
         <v>19</v>
       </c>
@@ -1946,8 +1956,8 @@
       <c r="A39" s="10">
         <v>37</v>
       </c>
-      <c r="B39" s="88"/>
-      <c r="C39" s="83"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="73"/>
       <c r="D39" s="48" t="s">
         <v>55</v>
       </c>
@@ -1967,8 +1977,8 @@
       <c r="A40" s="10">
         <v>38</v>
       </c>
-      <c r="B40" s="88"/>
-      <c r="C40" s="82" t="s">
+      <c r="B40" s="75"/>
+      <c r="C40" s="71" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="49" t="s">
@@ -1990,8 +2000,8 @@
       <c r="A41" s="10">
         <v>39</v>
       </c>
-      <c r="B41" s="88"/>
-      <c r="C41" s="90"/>
+      <c r="B41" s="75"/>
+      <c r="C41" s="72"/>
       <c r="D41" s="48" t="s">
         <v>19</v>
       </c>
@@ -2011,8 +2021,8 @@
       <c r="A42" s="10">
         <v>40</v>
       </c>
-      <c r="B42" s="89"/>
-      <c r="C42" s="83"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="73"/>
       <c r="D42" s="48" t="s">
         <v>55</v>
       </c>
@@ -2051,10 +2061,10 @@
       <c r="A44" s="10">
         <v>42</v>
       </c>
-      <c r="B44" s="87" t="s">
+      <c r="B44" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="82" t="s">
+      <c r="C44" s="71" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="49" t="s">
@@ -2076,8 +2086,8 @@
       <c r="A45" s="10">
         <v>43</v>
       </c>
-      <c r="B45" s="88"/>
-      <c r="C45" s="83"/>
+      <c r="B45" s="75"/>
+      <c r="C45" s="73"/>
       <c r="D45" s="48" t="s">
         <v>55</v>
       </c>
@@ -2097,8 +2107,8 @@
       <c r="A46" s="10">
         <v>44</v>
       </c>
-      <c r="B46" s="88"/>
-      <c r="C46" s="82" t="s">
+      <c r="B46" s="75"/>
+      <c r="C46" s="71" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="49" t="s">
@@ -2120,8 +2130,8 @@
       <c r="A47" s="10">
         <v>45</v>
       </c>
-      <c r="B47" s="88"/>
-      <c r="C47" s="90"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="72"/>
       <c r="D47" s="49" t="s">
         <v>71</v>
       </c>
@@ -2141,8 +2151,8 @@
       <c r="A48" s="10">
         <v>46</v>
       </c>
-      <c r="B48" s="88"/>
-      <c r="C48" s="83"/>
+      <c r="B48" s="75"/>
+      <c r="C48" s="73"/>
       <c r="D48" s="48" t="s">
         <v>55</v>
       </c>
@@ -2162,8 +2172,8 @@
       <c r="A49" s="10">
         <v>47</v>
       </c>
-      <c r="B49" s="88"/>
-      <c r="C49" s="82" t="s">
+      <c r="B49" s="75"/>
+      <c r="C49" s="71" t="s">
         <v>24</v>
       </c>
       <c r="D49" s="49" t="s">
@@ -2185,8 +2195,8 @@
       <c r="A50" s="10">
         <v>48</v>
       </c>
-      <c r="B50" s="88"/>
-      <c r="C50" s="90"/>
+      <c r="B50" s="75"/>
+      <c r="C50" s="72"/>
       <c r="D50" s="49" t="s">
         <v>26</v>
       </c>
@@ -2206,8 +2216,8 @@
       <c r="A51" s="10">
         <v>49</v>
       </c>
-      <c r="B51" s="88"/>
-      <c r="C51" s="83"/>
+      <c r="B51" s="75"/>
+      <c r="C51" s="73"/>
       <c r="D51" s="48" t="s">
         <v>55</v>
       </c>
@@ -2227,8 +2237,8 @@
       <c r="A52" s="10">
         <v>50</v>
       </c>
-      <c r="B52" s="88"/>
-      <c r="C52" s="82" t="s">
+      <c r="B52" s="75"/>
+      <c r="C52" s="71" t="s">
         <v>27</v>
       </c>
       <c r="D52" s="48" t="s">
@@ -2250,8 +2260,8 @@
       <c r="A53" s="10">
         <v>51</v>
       </c>
-      <c r="B53" s="89"/>
-      <c r="C53" s="83"/>
+      <c r="B53" s="76"/>
+      <c r="C53" s="73"/>
       <c r="D53" s="48" t="s">
         <v>29</v>
       </c>
@@ -2290,7 +2300,7 @@
       <c r="A55" s="10">
         <v>53</v>
       </c>
-      <c r="B55" s="73" t="s">
+      <c r="B55" s="92" t="s">
         <v>30</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -2315,7 +2325,7 @@
       <c r="A56" s="10">
         <v>54</v>
       </c>
-      <c r="B56" s="74"/>
+      <c r="B56" s="93"/>
       <c r="C56" s="7" t="s">
         <v>33</v>
       </c>
@@ -2338,7 +2348,7 @@
       <c r="A57" s="10">
         <v>55</v>
       </c>
-      <c r="B57" s="74"/>
+      <c r="B57" s="93"/>
       <c r="C57" s="7" t="s">
         <v>35</v>
       </c>
@@ -2361,7 +2371,7 @@
       <c r="A58" s="10">
         <v>56</v>
       </c>
-      <c r="B58" s="75"/>
+      <c r="B58" s="94"/>
       <c r="C58" s="25"/>
       <c r="D58" s="48" t="s">
         <v>55</v>
@@ -2382,10 +2392,10 @@
       <c r="A59" s="10">
         <v>57</v>
       </c>
-      <c r="B59" s="73" t="s">
+      <c r="B59" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C59" s="82" t="s">
+      <c r="C59" s="71" t="s">
         <v>4</v>
       </c>
       <c r="D59" s="48" t="s">
@@ -2407,8 +2417,8 @@
       <c r="A60" s="10">
         <v>58</v>
       </c>
-      <c r="B60" s="74"/>
-      <c r="C60" s="83"/>
+      <c r="B60" s="93"/>
+      <c r="C60" s="73"/>
       <c r="D60" s="48" t="s">
         <v>60</v>
       </c>
@@ -2427,7 +2437,7 @@
       <c r="A61" s="10">
         <v>59</v>
       </c>
-      <c r="B61" s="74"/>
+      <c r="B61" s="93"/>
       <c r="C61" s="27" t="s">
         <v>37</v>
       </c>
@@ -2450,7 +2460,7 @@
       <c r="A62" s="10">
         <v>60</v>
       </c>
-      <c r="B62" s="74"/>
+      <c r="B62" s="93"/>
       <c r="C62" s="27" t="s">
         <v>38</v>
       </c>
@@ -2473,7 +2483,7 @@
       <c r="A63" s="10">
         <v>61</v>
       </c>
-      <c r="B63" s="74"/>
+      <c r="B63" s="93"/>
       <c r="C63" s="25"/>
       <c r="D63" s="48" t="s">
         <v>56</v>
@@ -2494,7 +2504,7 @@
       <c r="A64" s="10">
         <v>62</v>
       </c>
-      <c r="B64" s="75"/>
+      <c r="B64" s="94"/>
       <c r="C64" s="25"/>
       <c r="D64" s="48" t="s">
         <v>55</v>
@@ -2515,7 +2525,7 @@
       <c r="A65" s="10">
         <v>63</v>
       </c>
-      <c r="B65" s="73" t="s">
+      <c r="B65" s="92" t="s">
         <v>41</v>
       </c>
       <c r="C65" s="27" t="s">
@@ -2525,7 +2535,7 @@
         <v>7</v>
       </c>
       <c r="E65" s="38"/>
-      <c r="F65" s="76"/>
+      <c r="F65" s="95"/>
       <c r="G65" s="9"/>
       <c r="H65" s="18"/>
       <c r="I65" s="18"/>
@@ -2540,7 +2550,7 @@
       <c r="A66" s="10">
         <v>64</v>
       </c>
-      <c r="B66" s="74"/>
+      <c r="B66" s="93"/>
       <c r="C66" s="27" t="s">
         <v>37</v>
       </c>
@@ -2548,7 +2558,7 @@
         <v>7</v>
       </c>
       <c r="E66" s="38"/>
-      <c r="F66" s="77"/>
+      <c r="F66" s="96"/>
       <c r="G66" s="9"/>
       <c r="H66" s="18"/>
       <c r="I66" s="18"/>
@@ -2563,7 +2573,7 @@
       <c r="A67" s="10">
         <v>65</v>
       </c>
-      <c r="B67" s="74"/>
+      <c r="B67" s="93"/>
       <c r="C67" s="27" t="s">
         <v>38</v>
       </c>
@@ -2571,7 +2581,7 @@
         <v>7</v>
       </c>
       <c r="E67" s="38"/>
-      <c r="F67" s="78"/>
+      <c r="F67" s="97"/>
       <c r="G67" s="9"/>
       <c r="H67" s="18"/>
       <c r="I67" s="18"/>
@@ -2586,7 +2596,7 @@
       <c r="A68" s="10">
         <v>66</v>
       </c>
-      <c r="B68" s="74"/>
+      <c r="B68" s="93"/>
       <c r="C68" s="25"/>
       <c r="D68" s="48" t="s">
         <v>56</v>
@@ -2607,7 +2617,7 @@
       <c r="A69" s="10">
         <v>67</v>
       </c>
-      <c r="B69" s="75"/>
+      <c r="B69" s="94"/>
       <c r="C69" s="25"/>
       <c r="D69" s="48" t="s">
         <v>55</v>
@@ -2628,7 +2638,7 @@
       <c r="A70" s="10">
         <v>68</v>
       </c>
-      <c r="B70" s="73" t="s">
+      <c r="B70" s="92" t="s">
         <v>42</v>
       </c>
       <c r="C70" s="28" t="s">
@@ -2653,7 +2663,7 @@
       <c r="A71" s="10">
         <v>69</v>
       </c>
-      <c r="B71" s="74"/>
+      <c r="B71" s="93"/>
       <c r="C71" s="28" t="s">
         <v>37</v>
       </c>
@@ -2676,7 +2686,7 @@
       <c r="A72" s="10">
         <v>70</v>
       </c>
-      <c r="B72" s="74"/>
+      <c r="B72" s="93"/>
       <c r="C72" s="28" t="s">
         <v>38</v>
       </c>
@@ -2699,7 +2709,7 @@
       <c r="A73" s="10">
         <v>71</v>
       </c>
-      <c r="B73" s="74"/>
+      <c r="B73" s="93"/>
       <c r="C73" s="24"/>
       <c r="D73" s="48" t="s">
         <v>56</v>
@@ -2720,7 +2730,7 @@
       <c r="A74" s="10">
         <v>72</v>
       </c>
-      <c r="B74" s="75"/>
+      <c r="B74" s="94"/>
       <c r="C74" s="26"/>
       <c r="D74" s="48" t="s">
         <v>55</v>
@@ -2741,7 +2751,7 @@
       <c r="A75" s="10">
         <v>73</v>
       </c>
-      <c r="B75" s="73" t="s">
+      <c r="B75" s="92" t="s">
         <v>61</v>
       </c>
       <c r="C75" s="7" t="s">
@@ -2766,7 +2776,7 @@
       <c r="A76" s="10">
         <v>74</v>
       </c>
-      <c r="B76" s="74"/>
+      <c r="B76" s="93"/>
       <c r="C76" s="7" t="s">
         <v>63</v>
       </c>
@@ -2789,7 +2799,7 @@
       <c r="A77" s="10">
         <v>75</v>
       </c>
-      <c r="B77" s="74"/>
+      <c r="B77" s="93"/>
       <c r="C77" s="43"/>
       <c r="D77" s="49" t="s">
         <v>69</v>
@@ -2810,7 +2820,7 @@
       <c r="A78" s="10">
         <v>76</v>
       </c>
-      <c r="B78" s="75"/>
+      <c r="B78" s="94"/>
       <c r="C78" s="25"/>
       <c r="D78" s="48" t="s">
         <v>55</v>
@@ -2831,7 +2841,7 @@
       <c r="A79" s="10">
         <v>77</v>
       </c>
-      <c r="B79" s="73" t="s">
+      <c r="B79" s="92" t="s">
         <v>47</v>
       </c>
       <c r="C79" s="7" t="s">
@@ -2841,7 +2851,7 @@
         <v>66</v>
       </c>
       <c r="E79" s="38"/>
-      <c r="F79" s="76"/>
+      <c r="F79" s="95"/>
       <c r="G79" s="9"/>
       <c r="H79" s="18"/>
       <c r="I79" s="18"/>
@@ -2856,7 +2866,7 @@
       <c r="A80" s="10">
         <v>78</v>
       </c>
-      <c r="B80" s="74"/>
+      <c r="B80" s="93"/>
       <c r="C80" s="7" t="s">
         <v>57</v>
       </c>
@@ -2864,7 +2874,7 @@
         <v>66</v>
       </c>
       <c r="E80" s="38"/>
-      <c r="F80" s="77"/>
+      <c r="F80" s="96"/>
       <c r="G80" s="9"/>
       <c r="H80" s="18"/>
       <c r="I80" s="18"/>
@@ -2879,7 +2889,7 @@
       <c r="A81" s="10">
         <v>79</v>
       </c>
-      <c r="B81" s="74"/>
+      <c r="B81" s="93"/>
       <c r="C81" s="7" t="s">
         <v>54</v>
       </c>
@@ -2887,7 +2897,7 @@
         <v>66</v>
       </c>
       <c r="E81" s="38"/>
-      <c r="F81" s="78"/>
+      <c r="F81" s="97"/>
       <c r="G81" s="9"/>
       <c r="H81" s="18"/>
       <c r="I81" s="18"/>
@@ -2902,7 +2912,7 @@
       <c r="A82" s="10">
         <v>80</v>
       </c>
-      <c r="B82" s="75"/>
+      <c r="B82" s="94"/>
       <c r="C82" s="7" t="s">
         <v>65</v>
       </c>
@@ -2925,7 +2935,7 @@
       <c r="A83" s="10">
         <v>81</v>
       </c>
-      <c r="B83" s="79" t="s">
+      <c r="B83" s="98" t="s">
         <v>48</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -2950,7 +2960,7 @@
       <c r="A84" s="10">
         <v>82</v>
       </c>
-      <c r="B84" s="80"/>
+      <c r="B84" s="99"/>
       <c r="C84" s="4" t="s">
         <v>52</v>
       </c>
@@ -2973,7 +2983,7 @@
       <c r="A85" s="10">
         <v>83</v>
       </c>
-      <c r="B85" s="81"/>
+      <c r="B85" s="100"/>
       <c r="C85" s="4" t="s">
         <v>53</v>
       </c>
@@ -2998,27 +3008,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="B3:B21"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C15:C20"/>
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="B75:B78"/>
     <mergeCell ref="B79:B82"/>
@@ -3035,6 +3024,27 @@
     <mergeCell ref="B44:B53"/>
     <mergeCell ref="C52:C53"/>
     <mergeCell ref="C22:C27"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="B3:B21"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="C46:C48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
RTGS test scripts added .
</commit_message>
<xml_diff>
--- a/src/test/java/com/corpnet/testData/Transaction_Tracker/Transaction_Tracker.xlsx
+++ b/src/test/java/com/corpnet/testData/Transaction_Tracker/Transaction_Tracker.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t>Transaction Reference</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>290823143253353P</t>
+  </si>
+  <si>
+    <t>290823155416851P</t>
   </si>
 </sst>
 </file>
@@ -1313,15 +1319,21 @@
       <c r="D9" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="54" t="s">
+        <v>76</v>
+      </c>
       <c r="G9" s="13"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
@@ -1359,15 +1371,21 @@
       <c r="D11" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>76</v>
+      </c>
       <c r="G11" s="13"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="M11" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="10">

</xml_diff>

<commit_message>
Refactor code scripts added .
</commit_message>
<xml_diff>
--- a/src/test/java/com/corpnet/testData/Transaction_Tracker/Transaction_Tracker.xlsx
+++ b/src/test/java/com/corpnet/testData/Transaction_Tracker/Transaction_Tracker.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="103">
   <si>
     <t>Transaction Reference</t>
   </si>
@@ -272,6 +272,69 @@
   </si>
   <si>
     <t>180923104220358P</t>
+  </si>
+  <si>
+    <t>190923104039271P</t>
+  </si>
+  <si>
+    <t>2,596.00</t>
+  </si>
+  <si>
+    <t>190923110134823P</t>
+  </si>
+  <si>
+    <t>RTGS Single Transaction</t>
+  </si>
+  <si>
+    <t>041023104739348P</t>
+  </si>
+  <si>
+    <t>041023114905345P</t>
+  </si>
+  <si>
+    <t>081023111724389P</t>
+  </si>
+  <si>
+    <t>081023113057825P</t>
+  </si>
+  <si>
+    <t>081023113314459P</t>
+  </si>
+  <si>
+    <t>081023120223568P</t>
+  </si>
+  <si>
+    <t>081023122243433P</t>
+  </si>
+  <si>
+    <t>IFT Single Transaction</t>
+  </si>
+  <si>
+    <t>081023122443964P</t>
+  </si>
+  <si>
+    <t>081023122654655P</t>
+  </si>
+  <si>
+    <t>081023125140988P</t>
+  </si>
+  <si>
+    <t>081023125444127P</t>
+  </si>
+  <si>
+    <t>081023133911390P</t>
+  </si>
+  <si>
+    <t>081023153817961P</t>
+  </si>
+  <si>
+    <t>081023154033571P</t>
+  </si>
+  <si>
+    <t>081023154318114P</t>
+  </si>
+  <si>
+    <t>091023114001997P</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1253,9 @@
       <c r="D3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E3"/>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
       <c r="F3" s="54" t="s">
         <v>76</v>
       </c>
@@ -1201,7 +1266,7 @@
       <c r="K3" s="18"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1215,7 +1280,9 @@
       <c r="D4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="42"/>
+      <c r="E4" s="42" t="s">
+        <v>90</v>
+      </c>
       <c r="F4" s="54"/>
       <c r="G4" s="13"/>
       <c r="H4" s="18"/>
@@ -1223,7 +1290,9 @@
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
@@ -1236,7 +1305,9 @@
       <c r="D5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="64"/>
+      <c r="E5" s="64" t="s">
+        <v>91</v>
+      </c>
       <c r="F5" s="54"/>
       <c r="G5" s="15"/>
       <c r="H5" s="18"/>
@@ -1244,7 +1315,9 @@
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="M5" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
     </row>
@@ -1323,7 +1396,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="F9" s="54" t="s">
         <v>76</v>
@@ -1335,7 +1408,7 @@
       <c r="K9" s="18"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -1350,9 +1423,11 @@
         <v>6</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="42"/>
+        <v>100</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>76</v>
+      </c>
       <c r="G10" s="13"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
@@ -1375,7 +1450,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="F11" s="54" t="s">
         <v>76</v>
@@ -1387,7 +1462,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1465,7 +1540,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>76</v>
@@ -1491,15 +1566,21 @@
       <c r="D16" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="80"/>
-      <c r="F16" s="81"/>
+      <c r="E16" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="81" t="s">
+        <v>76</v>
+      </c>
       <c r="G16" s="88"/>
       <c r="H16" s="90"/>
       <c r="I16" s="90"/>
       <c r="J16" s="90"/>
       <c r="K16" s="90"/>
       <c r="L16" s="83"/>
-      <c r="M16" s="44"/>
+      <c r="M16" s="44" t="s">
+        <v>78</v>
+      </c>
       <c r="N16" s="83"/>
       <c r="O16" s="44"/>
     </row>

</xml_diff>